<commit_message>
JSON english and spanish
</commit_message>
<xml_diff>
--- a/ShowPT/Assets/Localization/localization.xlsx
+++ b/ShowPT/Assets/Localization/localization.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mizel\Documents\Out-aLive\ShowPT\Assets\Localization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Unity\Out aLive\ShowPT\Assets\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80131821-D771-428B-ADE7-D011CE01FC6F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="250">
   <si>
     <t>Start Menu</t>
   </si>
@@ -114,60 +110,27 @@
     <t xml:space="preserve">The contestant has just arrived at the Zone, </t>
   </si>
   <si>
-    <t>TV 1.0</t>
-  </si>
-  <si>
-    <t>TV 1.1</t>
-  </si>
-  <si>
     <t>let's hope he is well equipped because there is no going back.</t>
   </si>
   <si>
-    <t>TV 2.0</t>
-  </si>
-  <si>
     <t>The contestant has just arrived at the middle of the Zone.</t>
   </si>
   <si>
-    <t>TV 2.1</t>
-  </si>
-  <si>
     <t>His goal is close.</t>
   </si>
   <si>
-    <t>TV 3.0</t>
-  </si>
-  <si>
-    <t>TV 3.1</t>
-  </si>
-  <si>
     <t>We’re on the home stretch!</t>
   </si>
   <si>
     <t>Let’s see if the contestant is able to break that shield down!</t>
   </si>
   <si>
-    <t>TV 4.0</t>
-  </si>
-  <si>
     <t>The drones are down!</t>
   </si>
   <si>
-    <t>TV 4.1</t>
-  </si>
-  <si>
     <t>And here it is, the surprise of the season!</t>
   </si>
   <si>
-    <t>TV 5.0</t>
-  </si>
-  <si>
-    <t>TV 5.1</t>
-  </si>
-  <si>
-    <t>TV 5.2</t>
-  </si>
-  <si>
     <t>A round of applause for our guardian robot.</t>
   </si>
   <si>
@@ -178,18 +141,6 @@
   </si>
   <si>
     <t>That's it! Good shot!</t>
-  </si>
-  <si>
-    <t>TV Boss 1</t>
-  </si>
-  <si>
-    <t>TV Boss 2</t>
-  </si>
-  <si>
-    <t>TV Boss 3</t>
-  </si>
-  <si>
-    <t>TV Boss 4</t>
   </si>
   <si>
     <t>Very good! Another one destroyed.</t>
@@ -644,13 +595,199 @@
   </si>
   <si>
     <t>SHOOT</t>
+  </si>
+  <si>
+    <t>INTERMISION</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>SALIR AL MENU</t>
+  </si>
+  <si>
+    <t>PORTUGESE</t>
+  </si>
+  <si>
+    <t>TVBOSS 1</t>
+  </si>
+  <si>
+    <t>TVBoss 2</t>
+  </si>
+  <si>
+    <t>TVBoss 3</t>
+  </si>
+  <si>
+    <t>TVBoss 4</t>
+  </si>
+  <si>
+    <t>TV1.0</t>
+  </si>
+  <si>
+    <t>TV1.1</t>
+  </si>
+  <si>
+    <t>TV2.0</t>
+  </si>
+  <si>
+    <t>TV2.1</t>
+  </si>
+  <si>
+    <t>TV3.0</t>
+  </si>
+  <si>
+    <t>TV3.1</t>
+  </si>
+  <si>
+    <t>TV4.0</t>
+  </si>
+  <si>
+    <t>TV4.1</t>
+  </si>
+  <si>
+    <t>TV5.0</t>
+  </si>
+  <si>
+    <t>TV5.1</t>
+  </si>
+  <si>
+    <t>TV5.2</t>
+  </si>
+  <si>
+    <t>ENDV1</t>
+  </si>
+  <si>
+    <t>ENDV2</t>
+  </si>
+  <si>
+    <t>ENDV3</t>
+  </si>
+  <si>
+    <t>ENDV4</t>
+  </si>
+  <si>
+    <t>STARTV1</t>
+  </si>
+  <si>
+    <t>STARTV2</t>
+  </si>
+  <si>
+    <t>STARTV3</t>
+  </si>
+  <si>
+    <t>STARTV4</t>
+  </si>
+  <si>
+    <t>STARTV5</t>
+  </si>
+  <si>
+    <t>EVTTURRET</t>
+  </si>
+  <si>
+    <t>EVTLIL</t>
+  </si>
+  <si>
+    <t>TWT1</t>
+  </si>
+  <si>
+    <t>TWT2</t>
+  </si>
+  <si>
+    <t>TWT3</t>
+  </si>
+  <si>
+    <t>TWT4</t>
+  </si>
+  <si>
+    <t>TWT5</t>
+  </si>
+  <si>
+    <t>TWT6</t>
+  </si>
+  <si>
+    <t>TWT7</t>
+  </si>
+  <si>
+    <t>TWT8</t>
+  </si>
+  <si>
+    <t>TWT9</t>
+  </si>
+  <si>
+    <t>TWT10</t>
+  </si>
+  <si>
+    <t>TWT11</t>
+  </si>
+  <si>
+    <t>TWT12</t>
+  </si>
+  <si>
+    <t>TWT13</t>
+  </si>
+  <si>
+    <t>TWT14</t>
+  </si>
+  <si>
+    <t>TWT15</t>
+  </si>
+  <si>
+    <t>ADEATH1</t>
+  </si>
+  <si>
+    <t>ADEATH2</t>
+  </si>
+  <si>
+    <t>ADEATH3</t>
+  </si>
+  <si>
+    <t>ADEATH4</t>
+  </si>
+  <si>
+    <t>CONTROL</t>
+  </si>
+  <si>
+    <t>MENUPAUSE</t>
+  </si>
+  <si>
+    <t>STADISTICS</t>
+  </si>
+  <si>
+    <t>CHANGEWPN</t>
+  </si>
+  <si>
+    <t>QUITMAIN</t>
+  </si>
+  <si>
+    <t>GAMEMACH</t>
+  </si>
+  <si>
+    <t>DOOR</t>
+  </si>
+  <si>
+    <t>BLOCKED</t>
+  </si>
+  <si>
+    <t>FRIEDGE</t>
+  </si>
+  <si>
+    <t>TOILET</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>LIFT</t>
+  </si>
+  <si>
+    <t>LASERGUN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,6 +799,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -714,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -723,6 +868,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1039,38 +1187,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1"/>
-    <col min="4" max="4" width="55.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="67.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="1"/>
+    <col min="4" max="4" width="55.26171875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67.578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="70.5234375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1078,13 +1231,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1092,13 +1245,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1106,13 +1259,13 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1120,13 +1273,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1134,13 +1287,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1148,13 +1301,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1162,19 +1315,20 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1182,7 +1336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1190,13 +1344,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1204,14 +1358,17 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1222,7 +1379,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="49.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1393,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1407,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1255,7 +1421,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1266,842 +1435,1010 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>196</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>197</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>198</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>199</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>200</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>201</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>202</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>203</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>204</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>206</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="E43" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="E44" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="E45" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E75" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="D77" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D61" s="1" t="s">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="B78" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D62" s="1" t="s">
+      <c r="E78" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" s="1" t="s">
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="1" t="s">
+      <c r="D81" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D67" s="1" t="s">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D69" s="1" t="s">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D70" s="1" t="s">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D71" s="1" t="s">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D72" s="1" t="s">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D73" s="1" t="s">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D82" s="1" t="s">
+    </row>
+    <row r="88" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D83" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D84" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E84" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D85" s="1" t="s">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D86" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D87" s="1" t="s">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
+      <c r="E91" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="E96" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D90" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="98" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Added translation for controls Screens and added French and Deutsch
</commit_message>
<xml_diff>
--- a/ShowPT/Assets/Localization/localization.xlsx
+++ b/ShowPT/Assets/Localization/localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Unity\Out aLive\ShowPT\Assets\Localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E74747-8C66-490C-8314-DB2E3DC452EC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73885433-6EB8-4A56-8066-32D9D1DAF5BF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="621">
   <si>
     <t>Start Menu</t>
   </si>
@@ -1079,9 +1079,6 @@
     <t>LEGENDAS</t>
   </si>
   <si>
-    <t>ARABE</t>
-  </si>
-  <si>
     <t>بدء العرض</t>
   </si>
   <si>
@@ -1341,6 +1338,567 @@
   </si>
   <si>
     <t>التالي</t>
+  </si>
+  <si>
+    <t>عنوان فرعي</t>
+  </si>
+  <si>
+    <t>للشرب</t>
+  </si>
+  <si>
+    <t>استعمال</t>
+  </si>
+  <si>
+    <t>لعب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فك الحجب مع Likes </t>
+  </si>
+  <si>
+    <t>]مقف[</t>
+  </si>
+  <si>
+    <t>العربية</t>
+  </si>
+  <si>
+    <t>BEGINNE DIE SHOW</t>
+  </si>
+  <si>
+    <t>OPTIONEN</t>
+  </si>
+  <si>
+    <t>ABSPANN</t>
+  </si>
+  <si>
+    <t>AUSGANG ZUM DESKTOP</t>
+  </si>
+  <si>
+    <t>GRAFIK</t>
+  </si>
+  <si>
+    <t>KLANG</t>
+  </si>
+  <si>
+    <t>GENERELL</t>
+  </si>
+  <si>
+    <t>ZURÜCK</t>
+  </si>
+  <si>
+    <t>DRÜCKE DIE LEERTASTE ZUM ÜBERSPRINGEN</t>
+  </si>
+  <si>
+    <t>Damen und Herren! Willkommen zu der neuen Edition von out a Live!</t>
+  </si>
+  <si>
+    <t>Am heutigen programm, wird unser Kandidat gegen ein Maschinenarsenal kämpfen, entwickelt um alles umzubringen, was sich bewegt.</t>
+  </si>
+  <si>
+    <t>Wir haben mehrere roboter entwickelt, die das Leben unmöglich machen werden, das Objektiv ist simpel.</t>
+  </si>
+  <si>
+    <t>Zerstöre die fliegende Drone um die Tür zu entsperren, die unseren kandidaten zu dem boss room führen wird.</t>
+  </si>
+  <si>
+    <t>Wird er lebend herrauskommen? Lasst die Show beginnen!</t>
+  </si>
+  <si>
+    <t>Der Kandidat ist gerade in der Zone angekommen,</t>
+  </si>
+  <si>
+    <t>lasst uns hoffen er ist gut vorbereitet, denn es gibt kein zurück.</t>
+  </si>
+  <si>
+    <t>Der Kandidat ist gerade in der Mitte der Zone angekommen.</t>
+  </si>
+  <si>
+    <t>Sein Ziel ist nah</t>
+  </si>
+  <si>
+    <t>Wir sind am Ziel</t>
+  </si>
+  <si>
+    <t>Lasst uns sehen ob der Kandidat das Schild brechen kann!</t>
+  </si>
+  <si>
+    <t>Die Drohnen sind gefallen!</t>
+  </si>
+  <si>
+    <t>Alles was für den Kandidaten übrig ist, ist die letzte Challenge!</t>
+  </si>
+  <si>
+    <t>Und hier ist sie, die Überraschung der Saison!</t>
+  </si>
+  <si>
+    <t>Eine Runde Applause für unseren Beschützerroboter!</t>
+  </si>
+  <si>
+    <t>Lasst uns sehen, wie unser Kandidat damit fertig wird.</t>
+  </si>
+  <si>
+    <t>Gut gemacht! Toller Schuss!</t>
+  </si>
+  <si>
+    <t>Sehr gut! Noch einer zerstört!</t>
+  </si>
+  <si>
+    <t>Seht euch das an! Ich habe noch nie so einen determinierten Kandidaten gesehen!</t>
+  </si>
+  <si>
+    <t>Der arme Roboter bekommt ganz schön was auf die Nuss!</t>
+  </si>
+  <si>
+    <t>Meine Damen und Herren! Wie haben einen Gewinner!</t>
+  </si>
+  <si>
+    <t>Das wars für diese Edition von Out a Live!</t>
+  </si>
+  <si>
+    <t>Ich hoffe ihr habt einen schönen Abend!</t>
+  </si>
+  <si>
+    <t>Bis bald!</t>
+  </si>
+  <si>
+    <t>Riecht es etwa nach verbranntem?</t>
+  </si>
+  <si>
+    <t>Es sah so freundlich aus, oder?</t>
+  </si>
+  <si>
+    <t>Hey, kein Spaß! Er sah dumm und schäbig aus, aber er hat es bis zur Brücke geschafft!</t>
+  </si>
+  <si>
+    <t>Wohin geht dieser Typ ohne Waffe? Hol dir eine von der Maschine, Verrückter! xD</t>
+  </si>
+  <si>
+    <t>Autsch! Das tat sogar mir weh!</t>
+  </si>
+  <si>
+    <t>Fünf Türmchen zerstört! Woher bekommen die überhaupt das Geld für so ein Schwachsinn?</t>
+  </si>
+  <si>
+    <t>Er ist schnell! Er hat es geschafft fünf Kamikaze Roboter zu zerstören bevor sie in sein Gesicht geflogen sind!</t>
+  </si>
+  <si>
+    <t>Unsere Gesellschaft stellt neue Mitglieder ein! Bewirb dich jetzt und bekomm eine gratis Käppie!</t>
+  </si>
+  <si>
+    <t>Zehn Bälle zerstört! So solls sein! Ich fühle mich identifiziert!</t>
+  </si>
+  <si>
+    <t>Zwanzig von uns sind gefallen!! DU MONSTER Ò_Ó</t>
+  </si>
+  <si>
+    <t>Wir haben ihn fast!!! Es lebe die überlegene Roboterrasse!</t>
+  </si>
+  <si>
+    <t>Ich weiß nicht… Das kommt mir alles falsch vor…</t>
+  </si>
+  <si>
+    <t>Möchte jemand ein Pyramidenschema mit mir bauen?</t>
+  </si>
+  <si>
+    <t>Dies ist eine Errinerung daran, dass die Show keine Beerdigungskosten übernimmt.</t>
+  </si>
+  <si>
+    <t>Kaufe Showgüter von unserer offiziellen Website</t>
+  </si>
+  <si>
+    <t>Hätten sie C++ benutzt, wäre das alles erträglicher</t>
+  </si>
+  <si>
+    <t>Hättest du jemals gedacht, wir könnten unechte Charaktere in einer Virtuellen Welt sein?</t>
+  </si>
+  <si>
+    <t>Der hat nicht lange gemacht… Nächster!</t>
+  </si>
+  <si>
+    <t>Owww! Das hat weh getan!</t>
+  </si>
+  <si>
+    <t>Ach… Noch ein Kandidat raus… Mal sehen ob der nächste es besser macht!</t>
+  </si>
+  <si>
+    <t>Wir hatten schon angefangen ihn zu mögen, oder? Naja, lasst den nächsten Kandidaten rein!</t>
+  </si>
+  <si>
+    <t>KONTROLLE</t>
+  </si>
+  <si>
+    <t>MENÜ/PAUSE</t>
+  </si>
+  <si>
+    <t>STATISTIK</t>
+  </si>
+  <si>
+    <t>RENNEN</t>
+  </si>
+  <si>
+    <t>BÜCKEN</t>
+  </si>
+  <si>
+    <t>WAFFE WECHSELN</t>
+  </si>
+  <si>
+    <t>NACHLADEN</t>
+  </si>
+  <si>
+    <t>INTERAGIEREN</t>
+  </si>
+  <si>
+    <t>SPRINGEN</t>
+  </si>
+  <si>
+    <t>BEWEGEN</t>
+  </si>
+  <si>
+    <t>GUCKEN</t>
+  </si>
+  <si>
+    <t>SCHIEßEN</t>
+  </si>
+  <si>
+    <t>INTERVALL</t>
+  </si>
+  <si>
+    <t>WEITER</t>
+  </si>
+  <si>
+    <t>RAUS ZUM MENÜ</t>
+  </si>
+  <si>
+    <t>Spielmaschine</t>
+  </si>
+  <si>
+    <t>Tür</t>
+  </si>
+  <si>
+    <t>Blockiert</t>
+  </si>
+  <si>
+    <t>Kühlschrank</t>
+  </si>
+  <si>
+    <t>Toilette</t>
+  </si>
+  <si>
+    <t>Offen</t>
+  </si>
+  <si>
+    <t>Fahrstuhl</t>
+  </si>
+  <si>
+    <t>Trinken</t>
+  </si>
+  <si>
+    <t>Benutzen</t>
+  </si>
+  <si>
+    <t>Spielen</t>
+  </si>
+  <si>
+    <t>LASERPISTOLE</t>
+  </si>
+  <si>
+    <t>SCHROTFLINTE</t>
+  </si>
+  <si>
+    <t>KANNONE</t>
+  </si>
+  <si>
+    <t>LEBEN</t>
+  </si>
+  <si>
+    <t>MUNITION</t>
+  </si>
+  <si>
+    <t>LEER</t>
+  </si>
+  <si>
+    <t>KAUFEN</t>
+  </si>
+  <si>
+    <t>DAVOR</t>
+  </si>
+  <si>
+    <t>NÄCHSTER</t>
+  </si>
+  <si>
+    <t>ENSPERREN MIT LIKES</t>
+  </si>
+  <si>
+    <t>[GESPERRT]</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>DÉMARRE LE SHOW</t>
+  </si>
+  <si>
+    <t>CRÉDITS</t>
+  </si>
+  <si>
+    <t>SORTIE VERS BUREAU</t>
+  </si>
+  <si>
+    <t>GRAFIQUE</t>
+  </si>
+  <si>
+    <t>SON</t>
+  </si>
+  <si>
+    <t>ÉCRAN PLEIN</t>
+  </si>
+  <si>
+    <t>GÉNÉRAL</t>
+  </si>
+  <si>
+    <t>RETOUR</t>
+  </si>
+  <si>
+    <t>APPUIE LA TOUCHE ESPACE POUR PASSER</t>
+  </si>
+  <si>
+    <t>Mesdammes et Monsieurs! Bienvenus à la nouvelle édition de out a Live!</t>
+  </si>
+  <si>
+    <t>Au Programme d'aujourd'hui, notre candidat va se battre contre un arsenal de machines, consitué pour tuer tout se qui bouge.</t>
+  </si>
+  <si>
+    <t>Nous avons crées plusieurs robots, qui vont rendre la vue impossible, l'objectif est simple.</t>
+  </si>
+  <si>
+    <t>Détruit les drones volantes pour dévérouiller la porte, qui mènera nore canditat à la chambre du boss.</t>
+  </si>
+  <si>
+    <t>Va-t-il s'en sortir vivant? Que le show commence!</t>
+  </si>
+  <si>
+    <t>Le candidat est arrivé à la zone,</t>
+  </si>
+  <si>
+    <t>espèrons qu'ils soit bien préparé, car il n'y a pas de retour!</t>
+  </si>
+  <si>
+    <t>Le candidat est arrivé au milieu de la zone.</t>
+  </si>
+  <si>
+    <t>Son but est proche</t>
+  </si>
+  <si>
+    <t>Nous sommes à l'arrivée!</t>
+  </si>
+  <si>
+    <t>Voyons si le candidat peut détruite le bouclier!</t>
+  </si>
+  <si>
+    <t>Les Drohnes sont tombées!</t>
+  </si>
+  <si>
+    <t>Maintenant il ne reste plus que le dernier challenge!</t>
+  </si>
+  <si>
+    <t>Et voici la surprise de la saison!</t>
+  </si>
+  <si>
+    <t>On applaudit notre robot protecteur!</t>
+  </si>
+  <si>
+    <t>Voyons, comment notre candidat va s'en sortir.</t>
+  </si>
+  <si>
+    <t>Bravo! Bon tire!</t>
+  </si>
+  <si>
+    <t>Très bien! Encore un détruit!</t>
+  </si>
+  <si>
+    <t>Regardez-moi ca! Je n'ai jamais vu un candidat aussi déterminé!</t>
+  </si>
+  <si>
+    <t>Le pauvre robot se fait bien tabasser!</t>
+  </si>
+  <si>
+    <t>Mesdames et Monsieurs! Nous avons un gagnant!</t>
+  </si>
+  <si>
+    <t>Jusqu'ici avec notre edition de Out a Live!</t>
+  </si>
+  <si>
+    <t>J'espère que vous passerez une bonne soirée!</t>
+  </si>
+  <si>
+    <t>À bientôt!</t>
+  </si>
+  <si>
+    <t>Est-ce que ca sent le brûlé?</t>
+  </si>
+  <si>
+    <t>Il avait l'air sympa, non?</t>
+  </si>
+  <si>
+    <t>Hey, sans blagues! Il avait l'air bête et maladroit, mais il a réussi à arriver au pont!</t>
+  </si>
+  <si>
+    <t>Oú va ce mec sans arme? Vas t'en chercher une à la machine, espèce de fou! XD</t>
+  </si>
+  <si>
+    <t>Aie! Ca à m'a fait mal même à moi!</t>
+  </si>
+  <si>
+    <t>Cinc tourettes détruites! Oú est-ce qu'ils trouvent l'argent pour tant de bêtises?</t>
+  </si>
+  <si>
+    <t>Il est rapide! Il a détruit cinc robots kamikazes avant qu'ils lui explosent à la figure!</t>
+  </si>
+  <si>
+    <t>Notre sociétée emploie de nouveaux membres! Présente-toi et recois un bonnet gratuit!</t>
+  </si>
+  <si>
+    <t>Dix balles détruites! Trés bien! Je me sens identifiée!</t>
+  </si>
+  <si>
+    <t>Veint des notres sont morts!! MONSTRE Ò_Ó</t>
+  </si>
+  <si>
+    <t>Nous l'avont presque! Vive la rasse supérieure de robots!</t>
+  </si>
+  <si>
+    <t>je ne sais pas… Ca me parrait tout faux!</t>
+  </si>
+  <si>
+    <t>Quelqu'un veut-il consuire un schema de pyramides avec moi?</t>
+  </si>
+  <si>
+    <t>Nous voulons vous rappeller, que ce show ne payera pas pour les enterrements.</t>
+  </si>
+  <si>
+    <t>Achète des produits du show sur notre page web officielle.</t>
+  </si>
+  <si>
+    <t>Si vous auriez utilisé C++, ce serait plus supportable.</t>
+  </si>
+  <si>
+    <t>N'as-tu jamais pensé que nous pourrions être des charactères non-réels dans un monde virtuel?</t>
+  </si>
+  <si>
+    <t>Celui-la n'as pas fait longtemps…Au prochain!</t>
+  </si>
+  <si>
+    <t>Aiiiiie! Ca a fait mal!</t>
+  </si>
+  <si>
+    <t>Halala… Encore un candidat dehors… Voyons si le prochain se débroulleras mieux!</t>
+  </si>
+  <si>
+    <t>Nous avions déjà commencé à bien l'aimer, n'est ce pas? Bon, faites entrer le prochain candidat!</t>
+  </si>
+  <si>
+    <t>CONTROLE</t>
+  </si>
+  <si>
+    <t>STATISTIQUE</t>
+  </si>
+  <si>
+    <t>COURRIR</t>
+  </si>
+  <si>
+    <t>PENCHER</t>
+  </si>
+  <si>
+    <t>CHANGER D'ARMES</t>
+  </si>
+  <si>
+    <t>RECHARGER</t>
+  </si>
+  <si>
+    <t>SAUTER</t>
+  </si>
+  <si>
+    <t>BOUGER</t>
+  </si>
+  <si>
+    <t>REGARDER</t>
+  </si>
+  <si>
+    <t>TIRER</t>
+  </si>
+  <si>
+    <t>INTERVALE</t>
+  </si>
+  <si>
+    <t>CONTINUER</t>
+  </si>
+  <si>
+    <t>SORTIR AU MENU</t>
+  </si>
+  <si>
+    <t>Machine de jeu</t>
+  </si>
+  <si>
+    <t>Porte</t>
+  </si>
+  <si>
+    <t>Bloqué</t>
+  </si>
+  <si>
+    <t>Frigidaire</t>
+  </si>
+  <si>
+    <t>Ouvert</t>
+  </si>
+  <si>
+    <t>Assenseur</t>
+  </si>
+  <si>
+    <t>Boire</t>
+  </si>
+  <si>
+    <t>Utiliser</t>
+  </si>
+  <si>
+    <t>Jouer</t>
+  </si>
+  <si>
+    <t>PISTOLET LASER</t>
+  </si>
+  <si>
+    <t>FUSIL DE CHASSE</t>
+  </si>
+  <si>
+    <t>CANON</t>
+  </si>
+  <si>
+    <t>VIE</t>
+  </si>
+  <si>
+    <t>VIDE</t>
+  </si>
+  <si>
+    <t>ACHETER</t>
+  </si>
+  <si>
+    <t>AVANT</t>
+  </si>
+  <si>
+    <t>APRÈS</t>
+  </si>
+  <si>
+    <t>DEBLOQUER AVEC LIKES</t>
+  </si>
+  <si>
+    <t>[BLOQUÉ]</t>
+  </si>
+  <si>
+    <t>UNTERTITEL</t>
+  </si>
+  <si>
+    <t>SOUS-TITRES</t>
   </si>
 </sst>
 </file>
@@ -1783,25 +2341,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.83984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83984375" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="55.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="67.578125" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="70.62890625" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55.26171875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67.578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="70.62890625" style="1" customWidth="1"/>
     <col min="7" max="7" width="99.3125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11" style="1"/>
+    <col min="8" max="8" width="61.9453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="85.62890625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>146</v>
       </c>
@@ -1818,10 +2378,16 @@
         <v>185</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+        <v>440</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1838,10 +2404,16 @@
         <v>243</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>348</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1858,10 +2430,16 @@
         <v>244</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>349</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1878,10 +2456,16 @@
         <v>245</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>350</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1898,10 +2482,16 @@
         <v>246</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>351</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1918,10 +2508,16 @@
         <v>247</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>352</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1938,10 +2534,16 @@
         <v>248</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>353</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1958,10 +2560,16 @@
         <v>249</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>354</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1979,10 +2587,16 @@
         <v>250</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>355</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1999,10 +2613,16 @@
         <v>251</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>356</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2019,10 +2639,16 @@
         <v>252</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>357</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>344</v>
       </c>
@@ -2038,9 +2664,18 @@
       <c r="F12" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>205</v>
       </c>
@@ -2057,10 +2692,16 @@
         <v>320</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="49.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>358</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="49.15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>206</v>
       </c>
@@ -2077,10 +2718,16 @@
         <v>253</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>359</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>207</v>
       </c>
@@ -2097,10 +2744,16 @@
         <v>254</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>360</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>208</v>
       </c>
@@ -2117,10 +2770,16 @@
         <v>255</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>361</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>209</v>
       </c>
@@ -2137,11 +2796,17 @@
         <v>256</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>362</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>190</v>
       </c>
@@ -2158,10 +2823,16 @@
         <v>257</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>363</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>191</v>
       </c>
@@ -2178,10 +2849,16 @@
         <v>258</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>364</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>192</v>
       </c>
@@ -2198,10 +2875,16 @@
         <v>259</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>365</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>193</v>
       </c>
@@ -2218,10 +2901,16 @@
         <v>260</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>366</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>194</v>
       </c>
@@ -2238,10 +2927,16 @@
         <v>261</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>367</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>195</v>
       </c>
@@ -2258,10 +2953,16 @@
         <v>262</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>368</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>196</v>
       </c>
@@ -2278,10 +2979,16 @@
         <v>263</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>369</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>197</v>
       </c>
@@ -2298,10 +3005,16 @@
         <v>264</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>370</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>198</v>
       </c>
@@ -2318,10 +3031,16 @@
         <v>265</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>374</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>199</v>
       </c>
@@ -2338,10 +3057,16 @@
         <v>266</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>375</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>200</v>
       </c>
@@ -2358,10 +3083,16 @@
         <v>267</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>371</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>186</v>
       </c>
@@ -2378,10 +3109,16 @@
         <v>268</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>376</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>187</v>
       </c>
@@ -2398,10 +3135,16 @@
         <v>269</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>377</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>188</v>
       </c>
@@ -2418,10 +3161,16 @@
         <v>270</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>372</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>189</v>
       </c>
@@ -2438,11 +3187,17 @@
         <v>271</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>373</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>201</v>
       </c>
@@ -2459,10 +3214,16 @@
         <v>272</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>393</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>202</v>
       </c>
@@ -2479,10 +3240,16 @@
         <v>322</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>398</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>203</v>
       </c>
@@ -2499,10 +3266,16 @@
         <v>273</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>394</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>204</v>
       </c>
@@ -2519,13 +3292,19 @@
         <v>274</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>395</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>210</v>
       </c>
@@ -2542,10 +3321,16 @@
         <v>275</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>396</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>211</v>
       </c>
@@ -2562,11 +3347,17 @@
         <v>276</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>397</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>212</v>
       </c>
@@ -2583,10 +3374,16 @@
         <v>277</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>378</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
         <v>213</v>
       </c>
@@ -2603,10 +3400,16 @@
         <v>278</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>379</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>214</v>
       </c>
@@ -2623,10 +3426,16 @@
         <v>279</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>380</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>215</v>
       </c>
@@ -2643,10 +3452,16 @@
         <v>280</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>381</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>216</v>
       </c>
@@ -2663,10 +3478,16 @@
         <v>281</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>382</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>217</v>
       </c>
@@ -2683,10 +3504,16 @@
         <v>282</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>383</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>218</v>
       </c>
@@ -2703,10 +3530,16 @@
         <v>283</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>384</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>219</v>
       </c>
@@ -2723,10 +3556,16 @@
         <v>284</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>385</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
         <v>220</v>
       </c>
@@ -2743,10 +3582,16 @@
         <v>285</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>386</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
         <v>221</v>
       </c>
@@ -2763,10 +3608,16 @@
         <v>286</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>387</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
         <v>222</v>
       </c>
@@ -2783,10 +3634,16 @@
         <v>287</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>388</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
         <v>223</v>
       </c>
@@ -2803,10 +3660,16 @@
         <v>288</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>389</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>224</v>
       </c>
@@ -2823,10 +3686,16 @@
         <v>289</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>390</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>225</v>
       </c>
@@ -2843,10 +3712,16 @@
         <v>290</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>391</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>226</v>
       </c>
@@ -2863,11 +3738,17 @@
         <v>291</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>392</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>227</v>
       </c>
@@ -2884,10 +3765,16 @@
         <v>292</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>399</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>228</v>
       </c>
@@ -2904,10 +3791,16 @@
         <v>293</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>400</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>229</v>
       </c>
@@ -2924,10 +3817,16 @@
         <v>294</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>401</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>230</v>
       </c>
@@ -2944,11 +3843,17 @@
         <v>295</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>402</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>231</v>
       </c>
@@ -2965,10 +3870,16 @@
         <v>87</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>403</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>232</v>
       </c>
@@ -2985,10 +3896,16 @@
         <v>296</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>404</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>233</v>
       </c>
@@ -3005,10 +3922,16 @@
         <v>297</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>405</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>173</v>
       </c>
@@ -3025,10 +3948,16 @@
         <v>90</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>406</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>174</v>
       </c>
@@ -3045,10 +3974,16 @@
         <v>298</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>407</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>234</v>
       </c>
@@ -3065,10 +4000,16 @@
         <v>299</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>408</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>176</v>
       </c>
@@ -3085,10 +4026,16 @@
         <v>300</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>409</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>177</v>
       </c>
@@ -3105,10 +4052,16 @@
         <v>301</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>410</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>178</v>
       </c>
@@ -3125,10 +4078,16 @@
         <v>302</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>411</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>179</v>
       </c>
@@ -3145,10 +4104,16 @@
         <v>303</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>412</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>180</v>
       </c>
@@ -3165,10 +4130,16 @@
         <v>304</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>413</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>181</v>
       </c>
@@ -3185,11 +4156,17 @@
         <v>305</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>414</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>182</v>
       </c>
@@ -3206,10 +4183,16 @@
         <v>306</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>415</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>100</v>
       </c>
@@ -3226,10 +4209,16 @@
         <v>183</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>416</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>235</v>
       </c>
@@ -3246,11 +4235,17 @@
         <v>307</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>417</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>236</v>
       </c>
@@ -3267,10 +4262,16 @@
         <v>308</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>418</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>237</v>
       </c>
@@ -3287,10 +4288,16 @@
         <v>309</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>419</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>238</v>
       </c>
@@ -3307,10 +4314,16 @@
         <v>113</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>420</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>341</v>
       </c>
@@ -3327,10 +4340,16 @@
         <v>310</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>421</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
         <v>239</v>
       </c>
@@ -3347,10 +4366,16 @@
         <v>311</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>422</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
         <v>240</v>
       </c>
@@ -3367,10 +4392,16 @@
         <v>116</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>423</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
         <v>241</v>
       </c>
@@ -3387,10 +4418,16 @@
         <v>312</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>424</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
         <v>331</v>
       </c>
@@ -3406,8 +4443,17 @@
       <c r="F89" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G89" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
         <v>332</v>
       </c>
@@ -3423,8 +4469,17 @@
       <c r="F90" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G90" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
         <v>337</v>
       </c>
@@ -3440,9 +4495,18 @@
       <c r="F91" s="1" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G91" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>242</v>
       </c>
@@ -3459,10 +4523,16 @@
         <v>313</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>425</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>327</v>
       </c>
@@ -3479,10 +4549,16 @@
         <v>130</v>
       </c>
       <c r="G94" s="7" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>426</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>132</v>
       </c>
@@ -3499,10 +4575,16 @@
         <v>314</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>427</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
         <v>134</v>
       </c>
@@ -3519,10 +4601,16 @@
         <v>133</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>428</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
         <v>136</v>
       </c>
@@ -3539,10 +4627,16 @@
         <v>315</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>429</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
         <v>138</v>
       </c>
@@ -3559,10 +4653,16 @@
         <v>316</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>430</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
         <v>140</v>
       </c>
@@ -3579,10 +4679,16 @@
         <v>139</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>431</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
         <v>143</v>
       </c>
@@ -3599,10 +4705,16 @@
         <v>141</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>432</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
         <v>144</v>
       </c>
@@ -3619,10 +4731,16 @@
         <v>317</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>433</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
         <v>323</v>
       </c>
@@ -3638,8 +4756,17 @@
       <c r="F102" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G102" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1" t="s">
         <v>328</v>
       </c>
@@ -3655,8 +4782,17 @@
       <c r="F103" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+      <c r="G103" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>